<commit_message>
16 july 2025 - Initial
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046981_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheSellsideDeals_NeitherSubjectNorBuyerIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046981_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheSellsideDeals_NeitherSubjectNorBuyerIsAPotentialRoundTrip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB86043-6116-4EAB-B0A2-C1A83275E8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83929E2-353A-4E3C-80EF-D45476250EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="568" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,7 +360,7 @@
     <t>FFL Partners LP</t>
   </si>
   <si>
-    <t>The Subject in this engagement satisfies the requirements of a round trip. If this subject is worth pursuing as a round trip candidate, please change the value to "Subject is a round trip".</t>
+    <t>The Subject in this engagement satisfies the requirements of a round trip. If this Subject is worth pursuing as a round trip candidate, please change the value to "Subject is a round trip".</t>
   </si>
 </sst>
 </file>
@@ -939,7 +939,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>